<commit_message>
add technician to validation list
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_preparation_v4_4_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_preparation_v4_4_0.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Library Batch" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Library" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Info" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Index" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Library Batch" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Library" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Info" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Index" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="Agilent_SureSelect_XT_V2_384" vbProcedure="false">Index!$W$2:$W$385</definedName>
@@ -11743,123 +11743,17 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12023,7 +11917,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -21295,7 +21189,7 @@
   <mergeCells count="1">
     <mergeCell ref="F5:H5"/>
   </mergeCells>
-  <dataValidations count="8">
+  <dataValidations count="9">
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B380" type="list">
       <formula1>Index!$E$2:$E$8</formula1>
       <formula2>0</formula2>
@@ -21324,8 +21218,12 @@
       <formula1>Index!$I$2:$I$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F7:G380" type="list">
-      <formula1>Index!$F$2:$F$9</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F7:F380" type="list">
+      <formula1>Index!$F$2:$F$10</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G7:G380" type="list">
+      <formula1>Index!$F$2:$F$10</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -21340,7 +21238,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -34182,7 +34080,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -35230,14 +35128,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AO1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added red asterisk to indicate that the container kind is mostly mandatory.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_preparation_v4_4_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_preparation_v4_4_0.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4690" uniqueCount="3701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4691" uniqueCount="3701">
   <si>
     <t xml:space="preserve">Library Preparation Template</t>
   </si>
@@ -21478,7 +21478,9 @@
         <v>3</v>
       </c>
       <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="H2" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>

</xml_diff>